<commit_message>
register, login, edit account, remove account done
</commit_message>
<xml_diff>
--- a/DOCS/WEB601-A2-CRUD-TABLE.xlsx
+++ b/DOCS/WEB601-A2-CRUD-TABLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\NMIT\WEB601\ws\WEB601-A2\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\36sli\Desktop\nmit\WEB-601\ws\WEB601-A2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1942A8A-AF87-487D-B74E-ACCADDFBDF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98429B-01A0-4431-9D6A-7CF416213EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8AE196B5-F491-4D70-B63D-C3E00D666E66}"/>
+    <workbookView xWindow="-15855" yWindow="4665" windowWidth="15855" windowHeight="13815" xr2:uid="{8AE196B5-F491-4D70-B63D-C3E00D666E66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,13 +307,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -887,156 +884,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0507DF9F-EDCC-436A-9743-46DC716AB5EA}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A5:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="18" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="18" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:18" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="11"/>
-      <c r="D7" s="13" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="8"/>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="O7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="11" t="s">
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="3"/>
@@ -1063,10 +1000,10 @@
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="8"/>
-    </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="11" t="s">
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="3"/>
@@ -1093,8 +1030,8 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="12" t="s">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="3"/>
@@ -1105,7 +1042,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>29</v>
@@ -1123,8 +1060,8 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="12" t="s">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="3"/>
@@ -1155,8 +1092,8 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="11" t="s">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1179,8 +1116,8 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="11" t="s">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1203,8 +1140,8 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="11" t="s">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1227,8 +1164,8 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="11" t="s">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3"/>
@@ -1255,8 +1192,8 @@
       </c>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="11" t="s">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="3"/>
@@ -1281,8 +1218,8 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="11" t="s">
+    <row r="17" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1309,8 +1246,8 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="11" t="s">
+    <row r="18" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="3"/>
@@ -1335,8 +1272,8 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="11" t="s">
+    <row r="19" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="3"/>
@@ -1361,8 +1298,8 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="11" t="s">
+    <row r="20" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="3"/>

</xml_diff>